<commit_message>
change to b nazanin font
</commit_message>
<xml_diff>
--- a/PythonScripts/payment_plan_0.5.xlsx
+++ b/PythonScripts/payment_plan_0.5.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Soheil izadi\Desktop\TelegramBot\TelegramBot\TelegramBot\PythonScripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0031C76B-A62F-4E5B-8C57-152C5957DE89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6A06174-0A53-49E3-BACF-B6C1478A88E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -204,7 +204,7 @@
     <numFmt numFmtId="165" formatCode="_-[$AED]\ * #,##0.00_-;\-[$AED]\ * #,##0.00_-;_-[$AED]\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="166" formatCode="_-[$AED]\ * #,##0_-;\-[$AED]\ * #,##0_-;_-[$AED]\ * &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -222,14 +222,6 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -272,6 +264,33 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="B Nazanin"/>
+      <charset val="178"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="0"/>
+      <name val="B Nazanin"/>
+      <charset val="178"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="B Nazanin"/>
+      <charset val="178"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="21"/>
+      <color theme="0"/>
+      <name val="B Nazanin"/>
+      <charset val="178"/>
     </font>
   </fonts>
   <fills count="7">
@@ -487,7 +506,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -501,7 +520,7 @@
     <xf numFmtId="164" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="15" fontId="4" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="15" fontId="3" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
@@ -516,7 +535,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -529,9 +548,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -556,88 +572,88 @@
     <xf numFmtId="1" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="7" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="6" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1031,8 +1047,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0F1C609-B3D0-401B-A2BD-FABD6A9C1BBB}">
   <dimension ref="A4:F118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11:E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1046,81 +1062,76 @@
   <sheetData>
     <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="42"/>
-      <c r="C5" s="43" t="s">
+      <c r="B5" s="23"/>
+      <c r="C5" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="43"/>
-      <c r="E5" s="44"/>
+      <c r="D5" s="45"/>
+      <c r="E5" s="46"/>
     </row>
     <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="42"/>
-      <c r="C6" s="45"/>
-      <c r="D6" s="45"/>
-      <c r="E6" s="46"/>
+      <c r="B6" s="23"/>
+      <c r="C6" s="47"/>
+      <c r="D6" s="47"/>
+      <c r="E6" s="48"/>
     </row>
     <row r="7" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="42"/>
-      <c r="C7" s="47"/>
-      <c r="D7" s="47"/>
-      <c r="E7" s="48"/>
-    </row>
-    <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="49"/>
-      <c r="C8" s="49"/>
-      <c r="D8" s="49"/>
-      <c r="E8" s="49"/>
-    </row>
+      <c r="B7" s="23"/>
+      <c r="C7" s="49"/>
+      <c r="D7" s="49"/>
+      <c r="E7" s="50"/>
+    </row>
+    <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="9" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="50" t="s">
+      <c r="B9" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="51"/>
-      <c r="D9" s="34">
+      <c r="C9" s="44"/>
+      <c r="D9" s="30">
         <f>SUM(D11/80)*100</f>
         <v>1500000</v>
       </c>
-      <c r="E9" s="35"/>
+      <c r="E9" s="31"/>
     </row>
     <row r="10" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="50" t="s">
+      <c r="B10" s="43" t="s">
         <v>51</v>
       </c>
-      <c r="C10" s="51"/>
-      <c r="D10" s="36">
+      <c r="C10" s="44"/>
+      <c r="D10" s="32">
         <v>220213</v>
       </c>
-      <c r="E10" s="36"/>
+      <c r="E10" s="32"/>
     </row>
     <row r="11" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="50" t="s">
+      <c r="B11" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="51"/>
-      <c r="D11" s="37">
+      <c r="C11" s="44"/>
+      <c r="D11" s="33">
         <v>1200000</v>
       </c>
-      <c r="E11" s="37"/>
+      <c r="E11" s="33"/>
       <c r="F11" s="14"/>
     </row>
     <row r="12" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:6" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="A13" s="15" t="s">
+    <row r="13" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A13" s="42" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="15" t="s">
+      <c r="B13" s="42" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="15" t="s">
+      <c r="C13" s="42" t="s">
         <v>9</v>
       </c>
-      <c r="D13" s="15" t="s">
+      <c r="D13" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="E13" s="15" t="s">
+      <c r="E13" s="42" t="s">
         <v>48</v>
       </c>
-      <c r="F13" s="15" t="s">
+      <c r="F13" s="42" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1128,7 +1139,7 @@
       <c r="A14" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B14" s="23"/>
+      <c r="B14" s="22"/>
       <c r="C14" s="11"/>
       <c r="D14" s="11"/>
       <c r="E14" s="11"/>
@@ -1143,24 +1154,24 @@
       <c r="F15" s="25"/>
     </row>
     <row r="16" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="15" t="s">
+      <c r="A16" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="B16" s="32" t="s">
+      <c r="B16" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="32"/>
-      <c r="D16" s="15" t="s">
+      <c r="C16" s="36"/>
+      <c r="D16" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="E16" s="15" t="s">
+      <c r="E16" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="F16" s="15" t="s">
+      <c r="F16" s="42" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>1</v>
       </c>
@@ -1179,7 +1190,7 @@
         <v>45863</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>2</v>
       </c>
@@ -1199,7 +1210,7 @@
         <v>45894</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A19" s="6">
         <v>3</v>
       </c>
@@ -1219,7 +1230,7 @@
         <v>45925</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A20" s="6">
         <v>4</v>
       </c>
@@ -1239,7 +1250,7 @@
         <v>45955</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A21" s="6">
         <v>5</v>
       </c>
@@ -1259,7 +1270,7 @@
         <v>45986</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A22" s="9">
         <v>6</v>
       </c>
@@ -1279,7 +1290,7 @@
         <v>46016</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A23" s="6">
         <v>7</v>
       </c>
@@ -1299,7 +1310,7 @@
         <v>46047</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A24" s="6">
         <v>8</v>
       </c>
@@ -1319,7 +1330,7 @@
         <v>46078</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A25" s="6">
         <v>9</v>
       </c>
@@ -1339,7 +1350,7 @@
         <v>46106</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A26" s="9">
         <v>10</v>
       </c>
@@ -1359,7 +1370,7 @@
         <v>46137</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A27" s="6">
         <v>11</v>
       </c>
@@ -1379,7 +1390,7 @@
         <v>46167</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A28" s="6">
         <v>12</v>
       </c>
@@ -1399,7 +1410,7 @@
         <v>46198</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A29" s="6">
         <v>13</v>
       </c>
@@ -1419,7 +1430,7 @@
         <v>46228</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A30" s="9">
         <v>14</v>
       </c>
@@ -1439,7 +1450,7 @@
         <v>46259</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A31" s="6">
         <v>15</v>
       </c>
@@ -1459,7 +1470,7 @@
         <v>46290</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A32" s="6">
         <v>16</v>
       </c>
@@ -1479,7 +1490,7 @@
         <v>46320</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A33" s="6">
         <v>17</v>
       </c>
@@ -1499,7 +1510,7 @@
         <v>46351</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A34" s="9">
         <v>18</v>
       </c>
@@ -1519,7 +1530,7 @@
         <v>46381</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A35" s="6">
         <v>19</v>
       </c>
@@ -1539,7 +1550,7 @@
         <v>46412</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A36" s="6">
         <v>20</v>
       </c>
@@ -1559,7 +1570,7 @@
         <v>46443</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A37" s="6">
         <v>21</v>
       </c>
@@ -1579,7 +1590,7 @@
         <v>46471</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A38" s="9">
         <v>22</v>
       </c>
@@ -1599,7 +1610,7 @@
         <v>46502</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A39" s="6">
         <v>23</v>
       </c>
@@ -1619,7 +1630,7 @@
         <v>46532</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A40" s="6">
         <v>24</v>
       </c>
@@ -1639,7 +1650,7 @@
         <v>46563</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A41" s="6">
         <v>25</v>
       </c>
@@ -1659,7 +1670,7 @@
         <v>46593</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A42" s="9">
         <v>26</v>
       </c>
@@ -1679,7 +1690,7 @@
         <v>46624</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A43" s="6">
         <v>27</v>
       </c>
@@ -1699,7 +1710,7 @@
         <v>46655</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A44" s="6">
         <v>28</v>
       </c>
@@ -1719,7 +1730,7 @@
         <v>46685</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A45" s="6">
         <v>33</v>
       </c>
@@ -1739,7 +1750,7 @@
         <v>46716</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A46" s="6">
         <v>34</v>
       </c>
@@ -1759,7 +1770,7 @@
         <v>46746</v>
       </c>
     </row>
-    <row r="47" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A47" s="6">
         <v>35</v>
       </c>
@@ -1779,7 +1790,7 @@
         <v>46777</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A48" s="9">
         <v>36</v>
       </c>
@@ -1799,7 +1810,7 @@
         <v>46808</v>
       </c>
     </row>
-    <row r="49" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A49" s="6">
         <v>37</v>
       </c>
@@ -1819,7 +1830,7 @@
         <v>46837</v>
       </c>
     </row>
-    <row r="50" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A50" s="6">
         <v>38</v>
       </c>
@@ -1839,7 +1850,7 @@
         <v>46868</v>
       </c>
     </row>
-    <row r="51" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A51" s="6">
         <v>39</v>
       </c>
@@ -1859,7 +1870,7 @@
         <v>46898</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A52" s="9">
         <v>40</v>
       </c>
@@ -1879,7 +1890,7 @@
         <v>46929</v>
       </c>
     </row>
-    <row r="53" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A53" s="6">
         <v>41</v>
       </c>
@@ -1899,7 +1910,7 @@
         <v>46959</v>
       </c>
     </row>
-    <row r="54" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A54" s="6">
         <v>42</v>
       </c>
@@ -1919,7 +1930,7 @@
         <v>46990</v>
       </c>
     </row>
-    <row r="55" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A55" s="6">
         <v>43</v>
       </c>
@@ -1939,7 +1950,7 @@
         <v>47021</v>
       </c>
     </row>
-    <row r="56" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A56" s="9">
         <v>44</v>
       </c>
@@ -1959,7 +1970,7 @@
         <v>47051</v>
       </c>
     </row>
-    <row r="57" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A57" s="6">
         <v>45</v>
       </c>
@@ -1979,7 +1990,7 @@
         <v>47082</v>
       </c>
     </row>
-    <row r="58" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A58" s="6">
         <v>46</v>
       </c>
@@ -1999,7 +2010,7 @@
         <v>47112</v>
       </c>
     </row>
-    <row r="59" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A59" s="6">
         <v>47</v>
       </c>
@@ -2019,7 +2030,7 @@
         <v>47143</v>
       </c>
     </row>
-    <row r="60" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A60" s="9">
         <v>48</v>
       </c>
@@ -2039,7 +2050,7 @@
         <v>47174</v>
       </c>
     </row>
-    <row r="61" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A61" s="6">
         <v>49</v>
       </c>
@@ -2059,7 +2070,7 @@
         <v>47202</v>
       </c>
     </row>
-    <row r="62" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A62" s="6">
         <v>50</v>
       </c>
@@ -2079,7 +2090,7 @@
         <v>47233</v>
       </c>
     </row>
-    <row r="63" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A63" s="6">
         <v>51</v>
       </c>
@@ -2099,7 +2110,7 @@
         <v>47263</v>
       </c>
     </row>
-    <row r="64" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A64" s="9">
         <v>52</v>
       </c>
@@ -2119,7 +2130,7 @@
         <v>47294</v>
       </c>
     </row>
-    <row r="65" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A65" s="6">
         <v>53</v>
       </c>
@@ -2139,7 +2150,7 @@
         <v>47324</v>
       </c>
     </row>
-    <row r="66" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A66" s="6">
         <v>54</v>
       </c>
@@ -2159,7 +2170,7 @@
         <v>47355</v>
       </c>
     </row>
-    <row r="67" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A67" s="6">
         <v>55</v>
       </c>
@@ -2179,7 +2190,7 @@
         <v>47386</v>
       </c>
     </row>
-    <row r="68" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A68" s="9">
         <v>56</v>
       </c>
@@ -2199,7 +2210,7 @@
         <v>47416</v>
       </c>
     </row>
-    <row r="69" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A69" s="6">
         <v>57</v>
       </c>
@@ -2219,7 +2230,7 @@
         <v>47447</v>
       </c>
     </row>
-    <row r="70" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A70" s="6">
         <v>58</v>
       </c>
@@ -2239,7 +2250,7 @@
         <v>47477</v>
       </c>
     </row>
-    <row r="71" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A71" s="6">
         <v>59</v>
       </c>
@@ -2259,7 +2270,7 @@
         <v>47508</v>
       </c>
     </row>
-    <row r="72" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A72" s="9">
         <v>60</v>
       </c>
@@ -2279,7 +2290,7 @@
         <v>47539</v>
       </c>
     </row>
-    <row r="73" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A73" s="6">
         <v>61</v>
       </c>
@@ -2299,7 +2310,7 @@
         <v>47567</v>
       </c>
     </row>
-    <row r="74" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A74" s="6">
         <v>62</v>
       </c>
@@ -2319,7 +2330,7 @@
         <v>47598</v>
       </c>
     </row>
-    <row r="75" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A75" s="6">
         <v>63</v>
       </c>
@@ -2356,190 +2367,190 @@
       <c r="F76" s="28"/>
     </row>
     <row r="78" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="31" t="s">
+      <c r="A78" s="35" t="s">
         <v>46</v>
       </c>
-      <c r="B78" s="32"/>
-      <c r="C78" s="32"/>
-      <c r="D78" s="32"/>
-      <c r="E78" s="32"/>
-      <c r="F78" s="33"/>
+      <c r="B78" s="36"/>
+      <c r="C78" s="36"/>
+      <c r="D78" s="36"/>
+      <c r="E78" s="36"/>
+      <c r="F78" s="37"/>
     </row>
     <row r="79" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="29" t="s">
+      <c r="A79" s="34" t="s">
         <v>47</v>
       </c>
-      <c r="B79" s="29"/>
+      <c r="B79" s="34"/>
       <c r="C79" s="6"/>
-      <c r="D79" s="30">
+      <c r="D79" s="29">
         <f>E76</f>
         <v>0</v>
       </c>
-      <c r="E79" s="30"/>
-      <c r="F79" s="30"/>
+      <c r="E79" s="29"/>
+      <c r="F79" s="29"/>
     </row>
     <row r="80" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="29" t="s">
+      <c r="A80" s="34" t="s">
         <v>49</v>
       </c>
-      <c r="B80" s="29"/>
+      <c r="B80" s="34"/>
       <c r="C80" s="6"/>
-      <c r="D80" s="30">
+      <c r="D80" s="29">
         <f>D79*4%</f>
         <v>0</v>
       </c>
-      <c r="E80" s="30"/>
-      <c r="F80" s="30"/>
+      <c r="E80" s="29"/>
+      <c r="F80" s="29"/>
     </row>
     <row r="81" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="29" t="s">
+      <c r="A81" s="34" t="s">
         <v>50</v>
       </c>
-      <c r="B81" s="29"/>
+      <c r="B81" s="34"/>
       <c r="C81" s="6"/>
-      <c r="D81" s="30">
+      <c r="D81" s="29">
         <v>4200</v>
       </c>
-      <c r="E81" s="30"/>
-      <c r="F81" s="30"/>
+      <c r="E81" s="29"/>
+      <c r="F81" s="29"/>
     </row>
     <row r="82" spans="1:6" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="20"/>
+      <c r="A82" s="19"/>
       <c r="D82" s="13"/>
       <c r="E82" s="13"/>
-      <c r="F82" s="16"/>
+      <c r="F82" s="15"/>
     </row>
     <row r="83" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="21"/>
-      <c r="F83" s="17"/>
+      <c r="A83" s="20"/>
+      <c r="F83" s="16"/>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A84" s="21"/>
-      <c r="F84" s="17"/>
+      <c r="A84" s="20"/>
+      <c r="F84" s="16"/>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A85" s="21"/>
-      <c r="F85" s="17"/>
+      <c r="A85" s="20"/>
+      <c r="F85" s="16"/>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A86" s="21"/>
-      <c r="F86" s="17"/>
+      <c r="A86" s="20"/>
+      <c r="F86" s="16"/>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A87" s="21"/>
-      <c r="F87" s="17"/>
+      <c r="A87" s="20"/>
+      <c r="F87" s="16"/>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A88" s="21"/>
-      <c r="F88" s="17"/>
+      <c r="A88" s="20"/>
+      <c r="F88" s="16"/>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A89" s="21"/>
-      <c r="F89" s="17"/>
+      <c r="A89" s="20"/>
+      <c r="F89" s="16"/>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A90" s="21"/>
-      <c r="F90" s="17"/>
+      <c r="A90" s="20"/>
+      <c r="F90" s="16"/>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A91" s="21"/>
-      <c r="F91" s="17"/>
+      <c r="A91" s="20"/>
+      <c r="F91" s="16"/>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A92" s="21"/>
-      <c r="F92" s="17"/>
+      <c r="A92" s="20"/>
+      <c r="F92" s="16"/>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A93" s="21"/>
-      <c r="F93" s="17"/>
+      <c r="A93" s="20"/>
+      <c r="F93" s="16"/>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A94" s="21"/>
-      <c r="F94" s="17"/>
+      <c r="A94" s="20"/>
+      <c r="F94" s="16"/>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A95" s="21"/>
-      <c r="F95" s="17"/>
+      <c r="A95" s="20"/>
+      <c r="F95" s="16"/>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A96" s="21"/>
-      <c r="F96" s="17"/>
+      <c r="A96" s="20"/>
+      <c r="F96" s="16"/>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A97" s="21"/>
-      <c r="F97" s="17"/>
+      <c r="A97" s="20"/>
+      <c r="F97" s="16"/>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A98" s="21"/>
-      <c r="F98" s="17"/>
+      <c r="A98" s="20"/>
+      <c r="F98" s="16"/>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A99" s="21"/>
-      <c r="F99" s="17"/>
+      <c r="A99" s="20"/>
+      <c r="F99" s="16"/>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A100" s="21"/>
-      <c r="F100" s="18"/>
+      <c r="A100" s="20"/>
+      <c r="F100" s="17"/>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A101" s="21"/>
-      <c r="F101" s="17"/>
+      <c r="A101" s="20"/>
+      <c r="F101" s="16"/>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A102" s="21"/>
-      <c r="F102" s="17"/>
+      <c r="A102" s="20"/>
+      <c r="F102" s="16"/>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A103" s="21"/>
-      <c r="F103" s="17"/>
+      <c r="A103" s="20"/>
+      <c r="F103" s="16"/>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A104" s="21"/>
-      <c r="F104" s="17"/>
+      <c r="A104" s="20"/>
+      <c r="F104" s="16"/>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A105" s="21"/>
-      <c r="F105" s="17"/>
+      <c r="A105" s="20"/>
+      <c r="F105" s="16"/>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A106" s="21"/>
-      <c r="F106" s="17"/>
+      <c r="A106" s="20"/>
+      <c r="F106" s="16"/>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A107" s="21"/>
-      <c r="F107" s="17"/>
+      <c r="A107" s="20"/>
+      <c r="F107" s="16"/>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A108" s="21"/>
-      <c r="F108" s="17"/>
+      <c r="A108" s="20"/>
+      <c r="F108" s="16"/>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A109" s="21"/>
-      <c r="F109" s="17"/>
+      <c r="A109" s="20"/>
+      <c r="F109" s="16"/>
     </row>
     <row r="110" spans="1:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="21"/>
-      <c r="F110" s="17"/>
+      <c r="A110" s="20"/>
+      <c r="F110" s="16"/>
     </row>
     <row r="111" spans="1:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="21"/>
-      <c r="F111" s="17"/>
+      <c r="A111" s="20"/>
+      <c r="F111" s="16"/>
     </row>
     <row r="112" spans="1:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="21"/>
-      <c r="F112" s="17"/>
+      <c r="A112" s="20"/>
+      <c r="F112" s="16"/>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A113" s="21"/>
-      <c r="F113" s="17"/>
+      <c r="A113" s="20"/>
+      <c r="F113" s="16"/>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A114" s="21"/>
-      <c r="F114" s="17"/>
+      <c r="A114" s="20"/>
+      <c r="F114" s="16"/>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A115" s="22"/>
-      <c r="F115" s="19"/>
+      <c r="A115" s="21"/>
+      <c r="F115" s="18"/>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116" s="24" t="s">
@@ -2569,6 +2580,68 @@
     </row>
   </sheetData>
   <mergeCells count="78">
+    <mergeCell ref="C5:E7"/>
+    <mergeCell ref="A116:F118"/>
+    <mergeCell ref="A15:F15"/>
+    <mergeCell ref="A76:B76"/>
+    <mergeCell ref="E76:F76"/>
+    <mergeCell ref="A80:B80"/>
+    <mergeCell ref="D80:F80"/>
+    <mergeCell ref="A81:B81"/>
+    <mergeCell ref="D81:F81"/>
+    <mergeCell ref="A78:F78"/>
+    <mergeCell ref="A79:B79"/>
+    <mergeCell ref="D79:F79"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="B75:C75"/>
+    <mergeCell ref="B69:C69"/>
+    <mergeCell ref="B70:C70"/>
+    <mergeCell ref="B71:C71"/>
+    <mergeCell ref="B72:C72"/>
+    <mergeCell ref="B73:C73"/>
     <mergeCell ref="B16:C16"/>
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="B10:C10"/>
@@ -2585,68 +2658,6 @@
     <mergeCell ref="B62:C62"/>
     <mergeCell ref="B63:C63"/>
     <mergeCell ref="B54:C54"/>
-    <mergeCell ref="B75:C75"/>
-    <mergeCell ref="B69:C69"/>
-    <mergeCell ref="B70:C70"/>
-    <mergeCell ref="B71:C71"/>
-    <mergeCell ref="B72:C72"/>
-    <mergeCell ref="B73:C73"/>
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="B56:C56"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="B58:C58"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="C5:E7"/>
-    <mergeCell ref="A116:F118"/>
-    <mergeCell ref="A15:F15"/>
-    <mergeCell ref="A76:B76"/>
-    <mergeCell ref="E76:F76"/>
-    <mergeCell ref="A80:B80"/>
-    <mergeCell ref="D80:F80"/>
-    <mergeCell ref="A81:B81"/>
-    <mergeCell ref="D81:F81"/>
-    <mergeCell ref="A78:F78"/>
-    <mergeCell ref="A79:B79"/>
-    <mergeCell ref="D79:F79"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="B17:C17"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <printOptions horizontalCentered="1"/>

</xml_diff>

<commit_message>
final fix for template
</commit_message>
<xml_diff>
--- a/PythonScripts/payment_plan_0.5.xlsx
+++ b/PythonScripts/payment_plan_0.5.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Soheil izadi\Desktop\TelegramBot\TelegramBot\TelegramBot\PythonScripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6A06174-0A53-49E3-BACF-B6C1478A88E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DFF7EC9-8978-49A7-A98D-5C16031B4C36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -186,13 +186,13 @@
     <t>مساحت کل به مترمربع</t>
   </si>
   <si>
-    <t>4% DLD (سازمان املاک و مستغلات)</t>
-  </si>
-  <si>
     <t>تنظیم قرارداد و امور اداری</t>
   </si>
   <si>
     <t>تخفیف ۲۰ درصد</t>
+  </si>
+  <si>
+    <t>4% DLD    سازمان املاک و مستغلات</t>
   </si>
 </sst>
 </file>
@@ -575,6 +575,27 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -590,9 +611,21 @@
     <xf numFmtId="164" fontId="5" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -605,18 +638,6 @@
     <xf numFmtId="166" fontId="6" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -629,31 +650,10 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1047,8 +1047,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0F1C609-B3D0-401B-A2BD-FABD6A9C1BBB}">
   <dimension ref="A4:F118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11:E11"/>
+    <sheetView tabSelected="1" topLeftCell="A76" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A80" sqref="A80:B80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1063,75 +1063,75 @@
     <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="23"/>
-      <c r="C5" s="45" t="s">
+      <c r="C5" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="45"/>
-      <c r="E5" s="46"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="26"/>
     </row>
     <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="23"/>
-      <c r="C6" s="47"/>
-      <c r="D6" s="47"/>
-      <c r="E6" s="48"/>
+      <c r="C6" s="27"/>
+      <c r="D6" s="27"/>
+      <c r="E6" s="28"/>
     </row>
     <row r="7" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="23"/>
-      <c r="C7" s="49"/>
-      <c r="D7" s="49"/>
-      <c r="E7" s="50"/>
+      <c r="C7" s="29"/>
+      <c r="D7" s="29"/>
+      <c r="E7" s="30"/>
     </row>
     <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="9" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="43" t="s">
+      <c r="B9" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="44"/>
-      <c r="D9" s="30">
+      <c r="C9" s="50"/>
+      <c r="D9" s="41">
         <f>SUM(D11/80)*100</f>
         <v>1500000</v>
       </c>
-      <c r="E9" s="31"/>
+      <c r="E9" s="42"/>
     </row>
     <row r="10" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="43" t="s">
-        <v>51</v>
-      </c>
-      <c r="C10" s="44"/>
-      <c r="D10" s="32">
+      <c r="B10" s="49" t="s">
+        <v>50</v>
+      </c>
+      <c r="C10" s="50"/>
+      <c r="D10" s="43">
         <v>220213</v>
       </c>
-      <c r="E10" s="32"/>
+      <c r="E10" s="43"/>
     </row>
     <row r="11" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="43" t="s">
+      <c r="B11" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="44"/>
-      <c r="D11" s="33">
+      <c r="C11" s="50"/>
+      <c r="D11" s="44">
         <v>1200000</v>
       </c>
-      <c r="E11" s="33"/>
+      <c r="E11" s="44"/>
       <c r="F11" s="14"/>
     </row>
     <row r="12" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="13" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A13" s="42" t="s">
+      <c r="A13" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="42" t="s">
+      <c r="B13" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="42" t="s">
+      <c r="C13" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="D13" s="42" t="s">
+      <c r="D13" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="E13" s="42" t="s">
+      <c r="E13" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="F13" s="42" t="s">
+      <c r="F13" s="24" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1146,28 +1146,28 @@
       <c r="F14" s="8"/>
     </row>
     <row r="15" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="25"/>
-      <c r="B15" s="25"/>
-      <c r="C15" s="25"/>
-      <c r="D15" s="25"/>
-      <c r="E15" s="25"/>
-      <c r="F15" s="25"/>
+      <c r="A15" s="32"/>
+      <c r="B15" s="32"/>
+      <c r="C15" s="32"/>
+      <c r="D15" s="32"/>
+      <c r="E15" s="32"/>
+      <c r="F15" s="32"/>
     </row>
     <row r="16" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="42" t="s">
+      <c r="A16" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="B16" s="36" t="s">
+      <c r="B16" s="39" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="36"/>
-      <c r="D16" s="42" t="s">
+      <c r="C16" s="39"/>
+      <c r="D16" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="E16" s="42" t="s">
+      <c r="E16" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="F16" s="42" t="s">
+      <c r="F16" s="24" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1175,10 +1175,10 @@
       <c r="A17" s="2">
         <v>1</v>
       </c>
-      <c r="B17" s="38" t="s">
+      <c r="B17" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="39"/>
+      <c r="C17" s="46"/>
       <c r="D17" s="3">
         <v>0.15</v>
       </c>
@@ -1194,10 +1194,10 @@
       <c r="A18" s="2">
         <v>2</v>
       </c>
-      <c r="B18" s="38" t="s">
+      <c r="B18" s="45" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="39"/>
+      <c r="C18" s="46"/>
       <c r="D18" s="3">
         <v>0.15</v>
       </c>
@@ -1214,10 +1214,10 @@
       <c r="A19" s="6">
         <v>3</v>
       </c>
-      <c r="B19" s="40" t="s">
+      <c r="B19" s="47" t="s">
         <v>18</v>
       </c>
-      <c r="C19" s="41"/>
+      <c r="C19" s="48"/>
       <c r="D19" s="7">
         <v>5.0000000000000001E-3</v>
       </c>
@@ -1234,10 +1234,10 @@
       <c r="A20" s="6">
         <v>4</v>
       </c>
-      <c r="B20" s="40" t="s">
+      <c r="B20" s="47" t="s">
         <v>19</v>
       </c>
-      <c r="C20" s="41"/>
+      <c r="C20" s="48"/>
       <c r="D20" s="7">
         <v>5.0000000000000001E-3</v>
       </c>
@@ -1254,10 +1254,10 @@
       <c r="A21" s="6">
         <v>5</v>
       </c>
-      <c r="B21" s="40" t="s">
+      <c r="B21" s="47" t="s">
         <v>20</v>
       </c>
-      <c r="C21" s="41"/>
+      <c r="C21" s="48"/>
       <c r="D21" s="7">
         <v>5.0000000000000001E-3</v>
       </c>
@@ -1274,10 +1274,10 @@
       <c r="A22" s="9">
         <v>6</v>
       </c>
-      <c r="B22" s="40" t="s">
+      <c r="B22" s="47" t="s">
         <v>21</v>
       </c>
-      <c r="C22" s="41"/>
+      <c r="C22" s="48"/>
       <c r="D22" s="7">
         <v>5.0000000000000001E-3</v>
       </c>
@@ -1294,10 +1294,10 @@
       <c r="A23" s="6">
         <v>7</v>
       </c>
-      <c r="B23" s="40" t="s">
+      <c r="B23" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="C23" s="41"/>
+      <c r="C23" s="48"/>
       <c r="D23" s="7">
         <v>5.0000000000000001E-3</v>
       </c>
@@ -1314,10 +1314,10 @@
       <c r="A24" s="6">
         <v>8</v>
       </c>
-      <c r="B24" s="40" t="s">
+      <c r="B24" s="47" t="s">
         <v>23</v>
       </c>
-      <c r="C24" s="41"/>
+      <c r="C24" s="48"/>
       <c r="D24" s="7">
         <v>5.0000000000000001E-3</v>
       </c>
@@ -1334,10 +1334,10 @@
       <c r="A25" s="6">
         <v>9</v>
       </c>
-      <c r="B25" s="40" t="s">
+      <c r="B25" s="47" t="s">
         <v>24</v>
       </c>
-      <c r="C25" s="41"/>
+      <c r="C25" s="48"/>
       <c r="D25" s="7">
         <v>5.0000000000000001E-3</v>
       </c>
@@ -1354,10 +1354,10 @@
       <c r="A26" s="9">
         <v>10</v>
       </c>
-      <c r="B26" s="40" t="s">
+      <c r="B26" s="47" t="s">
         <v>25</v>
       </c>
-      <c r="C26" s="41"/>
+      <c r="C26" s="48"/>
       <c r="D26" s="7">
         <v>5.0000000000000001E-3</v>
       </c>
@@ -1374,10 +1374,10 @@
       <c r="A27" s="6">
         <v>11</v>
       </c>
-      <c r="B27" s="40" t="s">
+      <c r="B27" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="C27" s="41"/>
+      <c r="C27" s="48"/>
       <c r="D27" s="7">
         <v>5.0000000000000001E-3</v>
       </c>
@@ -1394,10 +1394,10 @@
       <c r="A28" s="6">
         <v>12</v>
       </c>
-      <c r="B28" s="40" t="s">
+      <c r="B28" s="47" t="s">
         <v>27</v>
       </c>
-      <c r="C28" s="41"/>
+      <c r="C28" s="48"/>
       <c r="D28" s="7">
         <v>5.0000000000000001E-3</v>
       </c>
@@ -1414,10 +1414,10 @@
       <c r="A29" s="6">
         <v>13</v>
       </c>
-      <c r="B29" s="40" t="s">
+      <c r="B29" s="47" t="s">
         <v>28</v>
       </c>
-      <c r="C29" s="41"/>
+      <c r="C29" s="48"/>
       <c r="D29" s="7">
         <v>5.0000000000000001E-3</v>
       </c>
@@ -1434,10 +1434,10 @@
       <c r="A30" s="9">
         <v>14</v>
       </c>
-      <c r="B30" s="40" t="s">
+      <c r="B30" s="47" t="s">
         <v>29</v>
       </c>
-      <c r="C30" s="41"/>
+      <c r="C30" s="48"/>
       <c r="D30" s="7">
         <v>5.0000000000000001E-3</v>
       </c>
@@ -1454,10 +1454,10 @@
       <c r="A31" s="6">
         <v>15</v>
       </c>
-      <c r="B31" s="40" t="s">
+      <c r="B31" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="C31" s="41"/>
+      <c r="C31" s="48"/>
       <c r="D31" s="7">
         <v>5.0000000000000001E-3</v>
       </c>
@@ -1474,10 +1474,10 @@
       <c r="A32" s="6">
         <v>16</v>
       </c>
-      <c r="B32" s="40" t="s">
+      <c r="B32" s="47" t="s">
         <v>31</v>
       </c>
-      <c r="C32" s="41"/>
+      <c r="C32" s="48"/>
       <c r="D32" s="7">
         <v>5.0000000000000001E-3</v>
       </c>
@@ -1494,10 +1494,10 @@
       <c r="A33" s="6">
         <v>17</v>
       </c>
-      <c r="B33" s="40" t="s">
+      <c r="B33" s="47" t="s">
         <v>32</v>
       </c>
-      <c r="C33" s="41"/>
+      <c r="C33" s="48"/>
       <c r="D33" s="7">
         <v>5.0000000000000001E-3</v>
       </c>
@@ -1514,10 +1514,10 @@
       <c r="A34" s="9">
         <v>18</v>
       </c>
-      <c r="B34" s="40" t="s">
+      <c r="B34" s="47" t="s">
         <v>33</v>
       </c>
-      <c r="C34" s="41"/>
+      <c r="C34" s="48"/>
       <c r="D34" s="7">
         <v>5.0000000000000001E-3</v>
       </c>
@@ -1534,10 +1534,10 @@
       <c r="A35" s="6">
         <v>19</v>
       </c>
-      <c r="B35" s="40" t="s">
+      <c r="B35" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="C35" s="41"/>
+      <c r="C35" s="48"/>
       <c r="D35" s="7">
         <v>5.0000000000000001E-3</v>
       </c>
@@ -1554,10 +1554,10 @@
       <c r="A36" s="6">
         <v>20</v>
       </c>
-      <c r="B36" s="40" t="s">
+      <c r="B36" s="47" t="s">
         <v>35</v>
       </c>
-      <c r="C36" s="41"/>
+      <c r="C36" s="48"/>
       <c r="D36" s="7">
         <v>5.0000000000000001E-3</v>
       </c>
@@ -1574,10 +1574,10 @@
       <c r="A37" s="6">
         <v>21</v>
       </c>
-      <c r="B37" s="40" t="s">
+      <c r="B37" s="47" t="s">
         <v>36</v>
       </c>
-      <c r="C37" s="41"/>
+      <c r="C37" s="48"/>
       <c r="D37" s="7">
         <v>5.0000000000000001E-3</v>
       </c>
@@ -1594,10 +1594,10 @@
       <c r="A38" s="9">
         <v>22</v>
       </c>
-      <c r="B38" s="40" t="s">
+      <c r="B38" s="47" t="s">
         <v>37</v>
       </c>
-      <c r="C38" s="41"/>
+      <c r="C38" s="48"/>
       <c r="D38" s="7">
         <v>5.0000000000000001E-3</v>
       </c>
@@ -1614,10 +1614,10 @@
       <c r="A39" s="6">
         <v>23</v>
       </c>
-      <c r="B39" s="40" t="s">
+      <c r="B39" s="47" t="s">
         <v>38</v>
       </c>
-      <c r="C39" s="41"/>
+      <c r="C39" s="48"/>
       <c r="D39" s="7">
         <v>5.0000000000000001E-3</v>
       </c>
@@ -1634,10 +1634,10 @@
       <c r="A40" s="6">
         <v>24</v>
       </c>
-      <c r="B40" s="40" t="s">
+      <c r="B40" s="47" t="s">
         <v>39</v>
       </c>
-      <c r="C40" s="41"/>
+      <c r="C40" s="48"/>
       <c r="D40" s="7">
         <v>5.0000000000000001E-3</v>
       </c>
@@ -1654,10 +1654,10 @@
       <c r="A41" s="6">
         <v>25</v>
       </c>
-      <c r="B41" s="40" t="s">
+      <c r="B41" s="47" t="s">
         <v>40</v>
       </c>
-      <c r="C41" s="41"/>
+      <c r="C41" s="48"/>
       <c r="D41" s="7">
         <v>5.0000000000000001E-3</v>
       </c>
@@ -1674,10 +1674,10 @@
       <c r="A42" s="9">
         <v>26</v>
       </c>
-      <c r="B42" s="40" t="s">
+      <c r="B42" s="47" t="s">
         <v>41</v>
       </c>
-      <c r="C42" s="41"/>
+      <c r="C42" s="48"/>
       <c r="D42" s="7">
         <v>5.0000000000000001E-3</v>
       </c>
@@ -1694,10 +1694,10 @@
       <c r="A43" s="6">
         <v>27</v>
       </c>
-      <c r="B43" s="40" t="s">
+      <c r="B43" s="47" t="s">
         <v>42</v>
       </c>
-      <c r="C43" s="41"/>
+      <c r="C43" s="48"/>
       <c r="D43" s="7">
         <v>5.0000000000000001E-3</v>
       </c>
@@ -1714,10 +1714,10 @@
       <c r="A44" s="6">
         <v>28</v>
       </c>
-      <c r="B44" s="40" t="s">
+      <c r="B44" s="47" t="s">
         <v>43</v>
       </c>
-      <c r="C44" s="41"/>
+      <c r="C44" s="48"/>
       <c r="D44" s="7">
         <v>5.0000000000000001E-3</v>
       </c>
@@ -1734,10 +1734,10 @@
       <c r="A45" s="6">
         <v>33</v>
       </c>
-      <c r="B45" s="38" t="s">
+      <c r="B45" s="45" t="s">
         <v>44</v>
       </c>
-      <c r="C45" s="39"/>
+      <c r="C45" s="46"/>
       <c r="D45" s="7">
         <v>0.27</v>
       </c>
@@ -1754,10 +1754,10 @@
       <c r="A46" s="6">
         <v>34</v>
       </c>
-      <c r="B46" s="40" t="s">
-        <v>17</v>
-      </c>
-      <c r="C46" s="41"/>
+      <c r="B46" s="47" t="s">
+        <v>17</v>
+      </c>
+      <c r="C46" s="48"/>
       <c r="D46" s="7">
         <v>0.01</v>
       </c>
@@ -1774,10 +1774,10 @@
       <c r="A47" s="6">
         <v>35</v>
       </c>
-      <c r="B47" s="40" t="s">
-        <v>17</v>
-      </c>
-      <c r="C47" s="41"/>
+      <c r="B47" s="47" t="s">
+        <v>17</v>
+      </c>
+      <c r="C47" s="48"/>
       <c r="D47" s="7">
         <v>0.01</v>
       </c>
@@ -1794,10 +1794,10 @@
       <c r="A48" s="9">
         <v>36</v>
       </c>
-      <c r="B48" s="40" t="s">
-        <v>17</v>
-      </c>
-      <c r="C48" s="41"/>
+      <c r="B48" s="47" t="s">
+        <v>17</v>
+      </c>
+      <c r="C48" s="48"/>
       <c r="D48" s="7">
         <v>0.01</v>
       </c>
@@ -1814,10 +1814,10 @@
       <c r="A49" s="6">
         <v>37</v>
       </c>
-      <c r="B49" s="40" t="s">
-        <v>17</v>
-      </c>
-      <c r="C49" s="41"/>
+      <c r="B49" s="47" t="s">
+        <v>17</v>
+      </c>
+      <c r="C49" s="48"/>
       <c r="D49" s="7">
         <v>0.01</v>
       </c>
@@ -1834,10 +1834,10 @@
       <c r="A50" s="6">
         <v>38</v>
       </c>
-      <c r="B50" s="40" t="s">
-        <v>17</v>
-      </c>
-      <c r="C50" s="41"/>
+      <c r="B50" s="47" t="s">
+        <v>17</v>
+      </c>
+      <c r="C50" s="48"/>
       <c r="D50" s="7">
         <v>0.01</v>
       </c>
@@ -1854,10 +1854,10 @@
       <c r="A51" s="6">
         <v>39</v>
       </c>
-      <c r="B51" s="40" t="s">
-        <v>17</v>
-      </c>
-      <c r="C51" s="41"/>
+      <c r="B51" s="47" t="s">
+        <v>17</v>
+      </c>
+      <c r="C51" s="48"/>
       <c r="D51" s="7">
         <v>0.01</v>
       </c>
@@ -1874,10 +1874,10 @@
       <c r="A52" s="9">
         <v>40</v>
       </c>
-      <c r="B52" s="40" t="s">
-        <v>17</v>
-      </c>
-      <c r="C52" s="41"/>
+      <c r="B52" s="47" t="s">
+        <v>17</v>
+      </c>
+      <c r="C52" s="48"/>
       <c r="D52" s="7">
         <v>0.01</v>
       </c>
@@ -1894,10 +1894,10 @@
       <c r="A53" s="6">
         <v>41</v>
       </c>
-      <c r="B53" s="40" t="s">
-        <v>17</v>
-      </c>
-      <c r="C53" s="41"/>
+      <c r="B53" s="47" t="s">
+        <v>17</v>
+      </c>
+      <c r="C53" s="48"/>
       <c r="D53" s="7">
         <v>0.01</v>
       </c>
@@ -1914,10 +1914,10 @@
       <c r="A54" s="6">
         <v>42</v>
       </c>
-      <c r="B54" s="40" t="s">
-        <v>17</v>
-      </c>
-      <c r="C54" s="41"/>
+      <c r="B54" s="47" t="s">
+        <v>17</v>
+      </c>
+      <c r="C54" s="48"/>
       <c r="D54" s="7">
         <v>0.01</v>
       </c>
@@ -1934,10 +1934,10 @@
       <c r="A55" s="6">
         <v>43</v>
       </c>
-      <c r="B55" s="40" t="s">
-        <v>17</v>
-      </c>
-      <c r="C55" s="41"/>
+      <c r="B55" s="47" t="s">
+        <v>17</v>
+      </c>
+      <c r="C55" s="48"/>
       <c r="D55" s="7">
         <v>0.01</v>
       </c>
@@ -1954,10 +1954,10 @@
       <c r="A56" s="9">
         <v>44</v>
       </c>
-      <c r="B56" s="40" t="s">
-        <v>17</v>
-      </c>
-      <c r="C56" s="41"/>
+      <c r="B56" s="47" t="s">
+        <v>17</v>
+      </c>
+      <c r="C56" s="48"/>
       <c r="D56" s="7">
         <v>0.01</v>
       </c>
@@ -1974,10 +1974,10 @@
       <c r="A57" s="6">
         <v>45</v>
       </c>
-      <c r="B57" s="40" t="s">
-        <v>17</v>
-      </c>
-      <c r="C57" s="41"/>
+      <c r="B57" s="47" t="s">
+        <v>17</v>
+      </c>
+      <c r="C57" s="48"/>
       <c r="D57" s="7">
         <v>0.01</v>
       </c>
@@ -1994,10 +1994,10 @@
       <c r="A58" s="6">
         <v>46</v>
       </c>
-      <c r="B58" s="40" t="s">
-        <v>17</v>
-      </c>
-      <c r="C58" s="41"/>
+      <c r="B58" s="47" t="s">
+        <v>17</v>
+      </c>
+      <c r="C58" s="48"/>
       <c r="D58" s="7">
         <v>0.01</v>
       </c>
@@ -2014,10 +2014,10 @@
       <c r="A59" s="6">
         <v>47</v>
       </c>
-      <c r="B59" s="40" t="s">
-        <v>17</v>
-      </c>
-      <c r="C59" s="41"/>
+      <c r="B59" s="47" t="s">
+        <v>17</v>
+      </c>
+      <c r="C59" s="48"/>
       <c r="D59" s="7">
         <v>0.01</v>
       </c>
@@ -2034,10 +2034,10 @@
       <c r="A60" s="9">
         <v>48</v>
       </c>
-      <c r="B60" s="40" t="s">
-        <v>17</v>
-      </c>
-      <c r="C60" s="41"/>
+      <c r="B60" s="47" t="s">
+        <v>17</v>
+      </c>
+      <c r="C60" s="48"/>
       <c r="D60" s="7">
         <v>0.01</v>
       </c>
@@ -2054,10 +2054,10 @@
       <c r="A61" s="6">
         <v>49</v>
       </c>
-      <c r="B61" s="40" t="s">
-        <v>17</v>
-      </c>
-      <c r="C61" s="41"/>
+      <c r="B61" s="47" t="s">
+        <v>17</v>
+      </c>
+      <c r="C61" s="48"/>
       <c r="D61" s="7">
         <v>0.01</v>
       </c>
@@ -2074,10 +2074,10 @@
       <c r="A62" s="6">
         <v>50</v>
       </c>
-      <c r="B62" s="40" t="s">
-        <v>17</v>
-      </c>
-      <c r="C62" s="41"/>
+      <c r="B62" s="47" t="s">
+        <v>17</v>
+      </c>
+      <c r="C62" s="48"/>
       <c r="D62" s="7">
         <v>0.01</v>
       </c>
@@ -2094,10 +2094,10 @@
       <c r="A63" s="6">
         <v>51</v>
       </c>
-      <c r="B63" s="40" t="s">
-        <v>17</v>
-      </c>
-      <c r="C63" s="41"/>
+      <c r="B63" s="47" t="s">
+        <v>17</v>
+      </c>
+      <c r="C63" s="48"/>
       <c r="D63" s="7">
         <v>0.01</v>
       </c>
@@ -2114,10 +2114,10 @@
       <c r="A64" s="9">
         <v>52</v>
       </c>
-      <c r="B64" s="40" t="s">
-        <v>17</v>
-      </c>
-      <c r="C64" s="41"/>
+      <c r="B64" s="47" t="s">
+        <v>17</v>
+      </c>
+      <c r="C64" s="48"/>
       <c r="D64" s="7">
         <v>0.01</v>
       </c>
@@ -2134,10 +2134,10 @@
       <c r="A65" s="6">
         <v>53</v>
       </c>
-      <c r="B65" s="40" t="s">
-        <v>17</v>
-      </c>
-      <c r="C65" s="41"/>
+      <c r="B65" s="47" t="s">
+        <v>17</v>
+      </c>
+      <c r="C65" s="48"/>
       <c r="D65" s="7">
         <v>0.01</v>
       </c>
@@ -2154,10 +2154,10 @@
       <c r="A66" s="6">
         <v>54</v>
       </c>
-      <c r="B66" s="40" t="s">
-        <v>17</v>
-      </c>
-      <c r="C66" s="41"/>
+      <c r="B66" s="47" t="s">
+        <v>17</v>
+      </c>
+      <c r="C66" s="48"/>
       <c r="D66" s="7">
         <v>0.01</v>
       </c>
@@ -2174,10 +2174,10 @@
       <c r="A67" s="6">
         <v>55</v>
       </c>
-      <c r="B67" s="40" t="s">
-        <v>17</v>
-      </c>
-      <c r="C67" s="41"/>
+      <c r="B67" s="47" t="s">
+        <v>17</v>
+      </c>
+      <c r="C67" s="48"/>
       <c r="D67" s="7">
         <v>0.01</v>
       </c>
@@ -2194,10 +2194,10 @@
       <c r="A68" s="9">
         <v>56</v>
       </c>
-      <c r="B68" s="40" t="s">
-        <v>17</v>
-      </c>
-      <c r="C68" s="41"/>
+      <c r="B68" s="47" t="s">
+        <v>17</v>
+      </c>
+      <c r="C68" s="48"/>
       <c r="D68" s="7">
         <v>0.01</v>
       </c>
@@ -2214,10 +2214,10 @@
       <c r="A69" s="6">
         <v>57</v>
       </c>
-      <c r="B69" s="40" t="s">
-        <v>17</v>
-      </c>
-      <c r="C69" s="41"/>
+      <c r="B69" s="47" t="s">
+        <v>17</v>
+      </c>
+      <c r="C69" s="48"/>
       <c r="D69" s="7">
         <v>0.01</v>
       </c>
@@ -2234,10 +2234,10 @@
       <c r="A70" s="6">
         <v>58</v>
       </c>
-      <c r="B70" s="40" t="s">
-        <v>17</v>
-      </c>
-      <c r="C70" s="41"/>
+      <c r="B70" s="47" t="s">
+        <v>17</v>
+      </c>
+      <c r="C70" s="48"/>
       <c r="D70" s="7">
         <v>0.01</v>
       </c>
@@ -2254,10 +2254,10 @@
       <c r="A71" s="6">
         <v>59</v>
       </c>
-      <c r="B71" s="40" t="s">
-        <v>17</v>
-      </c>
-      <c r="C71" s="41"/>
+      <c r="B71" s="47" t="s">
+        <v>17</v>
+      </c>
+      <c r="C71" s="48"/>
       <c r="D71" s="7">
         <v>0.01</v>
       </c>
@@ -2274,10 +2274,10 @@
       <c r="A72" s="9">
         <v>60</v>
       </c>
-      <c r="B72" s="40" t="s">
-        <v>17</v>
-      </c>
-      <c r="C72" s="41"/>
+      <c r="B72" s="47" t="s">
+        <v>17</v>
+      </c>
+      <c r="C72" s="48"/>
       <c r="D72" s="7">
         <v>0.01</v>
       </c>
@@ -2294,10 +2294,10 @@
       <c r="A73" s="6">
         <v>61</v>
       </c>
-      <c r="B73" s="40" t="s">
-        <v>17</v>
-      </c>
-      <c r="C73" s="41"/>
+      <c r="B73" s="47" t="s">
+        <v>17</v>
+      </c>
+      <c r="C73" s="48"/>
       <c r="D73" s="7">
         <v>0.01</v>
       </c>
@@ -2314,10 +2314,10 @@
       <c r="A74" s="6">
         <v>62</v>
       </c>
-      <c r="B74" s="40" t="s">
-        <v>17</v>
-      </c>
-      <c r="C74" s="41"/>
+      <c r="B74" s="47" t="s">
+        <v>17</v>
+      </c>
+      <c r="C74" s="48"/>
       <c r="D74" s="7">
         <v>0.01</v>
       </c>
@@ -2334,10 +2334,10 @@
       <c r="A75" s="6">
         <v>63</v>
       </c>
-      <c r="B75" s="40" t="s">
-        <v>17</v>
-      </c>
-      <c r="C75" s="41"/>
+      <c r="B75" s="47" t="s">
+        <v>17</v>
+      </c>
+      <c r="C75" s="48"/>
       <c r="D75" s="7">
         <v>0.01</v>
       </c>
@@ -2351,68 +2351,68 @@
       </c>
     </row>
     <row r="76" spans="1:6" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="A76" s="26" t="s">
+      <c r="A76" s="33" t="s">
         <v>45</v>
       </c>
-      <c r="B76" s="26"/>
+      <c r="B76" s="33"/>
       <c r="C76" s="10"/>
       <c r="D76" s="12">
         <f>SUM(D17:D75)</f>
         <v>1.0000000000000004</v>
       </c>
-      <c r="E76" s="27">
+      <c r="E76" s="34">
         <f>SUM(E17:E75)</f>
         <v>0</v>
       </c>
-      <c r="F76" s="28"/>
+      <c r="F76" s="35"/>
     </row>
     <row r="78" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="35" t="s">
+      <c r="A78" s="38" t="s">
         <v>46</v>
       </c>
-      <c r="B78" s="36"/>
-      <c r="C78" s="36"/>
-      <c r="D78" s="36"/>
-      <c r="E78" s="36"/>
-      <c r="F78" s="37"/>
+      <c r="B78" s="39"/>
+      <c r="C78" s="39"/>
+      <c r="D78" s="39"/>
+      <c r="E78" s="39"/>
+      <c r="F78" s="40"/>
     </row>
     <row r="79" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="34" t="s">
+      <c r="A79" s="36" t="s">
         <v>47</v>
       </c>
-      <c r="B79" s="34"/>
+      <c r="B79" s="36"/>
       <c r="C79" s="6"/>
-      <c r="D79" s="29">
+      <c r="D79" s="37">
         <f>E76</f>
         <v>0</v>
       </c>
-      <c r="E79" s="29"/>
-      <c r="F79" s="29"/>
+      <c r="E79" s="37"/>
+      <c r="F79" s="37"/>
     </row>
     <row r="80" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="34" t="s">
+      <c r="A80" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="B80" s="36"/>
+      <c r="C80" s="6"/>
+      <c r="D80" s="37">
+        <f>D79*4%</f>
+        <v>0</v>
+      </c>
+      <c r="E80" s="37"/>
+      <c r="F80" s="37"/>
+    </row>
+    <row r="81" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="36" t="s">
         <v>49</v>
       </c>
-      <c r="B80" s="34"/>
-      <c r="C80" s="6"/>
-      <c r="D80" s="29">
-        <f>D79*4%</f>
-        <v>0</v>
-      </c>
-      <c r="E80" s="29"/>
-      <c r="F80" s="29"/>
-    </row>
-    <row r="81" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="34" t="s">
-        <v>50</v>
-      </c>
-      <c r="B81" s="34"/>
+      <c r="B81" s="36"/>
       <c r="C81" s="6"/>
-      <c r="D81" s="29">
+      <c r="D81" s="37">
         <v>4200</v>
       </c>
-      <c r="E81" s="29"/>
-      <c r="F81" s="29"/>
+      <c r="E81" s="37"/>
+      <c r="F81" s="37"/>
     </row>
     <row r="82" spans="1:6" ht="6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="19"/>
@@ -2553,33 +2553,95 @@
       <c r="F115" s="18"/>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A116" s="24" t="s">
+      <c r="A116" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="B116" s="24"/>
-      <c r="C116" s="24"/>
-      <c r="D116" s="24"/>
-      <c r="E116" s="24"/>
-      <c r="F116" s="24"/>
+      <c r="B116" s="31"/>
+      <c r="C116" s="31"/>
+      <c r="D116" s="31"/>
+      <c r="E116" s="31"/>
+      <c r="F116" s="31"/>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A117" s="24"/>
-      <c r="B117" s="24"/>
-      <c r="C117" s="24"/>
-      <c r="D117" s="24"/>
-      <c r="E117" s="24"/>
-      <c r="F117" s="24"/>
+      <c r="A117" s="31"/>
+      <c r="B117" s="31"/>
+      <c r="C117" s="31"/>
+      <c r="D117" s="31"/>
+      <c r="E117" s="31"/>
+      <c r="F117" s="31"/>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A118" s="24"/>
-      <c r="B118" s="24"/>
-      <c r="C118" s="24"/>
-      <c r="D118" s="24"/>
-      <c r="E118" s="24"/>
-      <c r="F118" s="24"/>
+      <c r="A118" s="31"/>
+      <c r="B118" s="31"/>
+      <c r="C118" s="31"/>
+      <c r="D118" s="31"/>
+      <c r="E118" s="31"/>
+      <c r="F118" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="78">
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B74:C74"/>
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="B67:C67"/>
+    <mergeCell ref="B68:C68"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="B60:C60"/>
+    <mergeCell ref="B61:C61"/>
+    <mergeCell ref="B62:C62"/>
+    <mergeCell ref="B63:C63"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="B75:C75"/>
+    <mergeCell ref="B69:C69"/>
+    <mergeCell ref="B70:C70"/>
+    <mergeCell ref="B71:C71"/>
+    <mergeCell ref="B72:C72"/>
+    <mergeCell ref="B73:C73"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
     <mergeCell ref="C5:E7"/>
     <mergeCell ref="A116:F118"/>
     <mergeCell ref="A15:F15"/>
@@ -2596,68 +2658,6 @@
     <mergeCell ref="D10:E10"/>
     <mergeCell ref="D11:E11"/>
     <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="B56:C56"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="B58:C58"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="B75:C75"/>
-    <mergeCell ref="B69:C69"/>
-    <mergeCell ref="B70:C70"/>
-    <mergeCell ref="B71:C71"/>
-    <mergeCell ref="B72:C72"/>
-    <mergeCell ref="B73:C73"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B74:C74"/>
-    <mergeCell ref="B64:C64"/>
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="B67:C67"/>
-    <mergeCell ref="B68:C68"/>
-    <mergeCell ref="B59:C59"/>
-    <mergeCell ref="B60:C60"/>
-    <mergeCell ref="B61:C61"/>
-    <mergeCell ref="B62:C62"/>
-    <mergeCell ref="B63:C63"/>
-    <mergeCell ref="B54:C54"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <printOptions horizontalCentered="1"/>

</xml_diff>